<commit_message>
Minimum approach temperature implemented for multiple single heat pump placement
</commit_message>
<xml_diff>
--- a/Excel_Version/Data_input_template.xlsx
+++ b/Excel_Version/Data_input_template.xlsx
@@ -1,21 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothyw/Github Local/OpenPinch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothyw/Github Local/OpenPinch/Excel_Version/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF40B97A-D5D9-D949-8F84-E24459DC996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306F13BF-845E-024A-B736-201033D91622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="1" xr2:uid="{BB0ED48D-3077-FB46-BBC1-F820D8E91AAE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="2" xr2:uid="{BB0ED48D-3077-FB46-BBC1-F820D8E91AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Stream Data" sheetId="1" r:id="rId1"/>
     <sheet name="Utility Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Options" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="a">#REF!</definedName>
+    <definedName name="b">#REF!</definedName>
+    <definedName name="c_0">#REF!</definedName>
+    <definedName name="configuration" localSheetId="2">Options!$A$1:$B$44</definedName>
+    <definedName name="Dev_01">#REF!</definedName>
+    <definedName name="Dev_02">#REF!</definedName>
+    <definedName name="Dev_03">#REF!</definedName>
+    <definedName name="Dev_04">#REF!</definedName>
+    <definedName name="Dev_05">#REF!</definedName>
+    <definedName name="Dev_06">#REF!</definedName>
+    <definedName name="Dev_11">[1]Derivatives!#REF!</definedName>
+    <definedName name="Diff_01">#REF!</definedName>
+    <definedName name="Diff_02">#REF!</definedName>
+    <definedName name="Diff_03">#REF!</definedName>
+    <definedName name="Diff_04">#REF!</definedName>
+    <definedName name="Diff_05">#REF!</definedName>
+    <definedName name="Diff_06">#REF!</definedName>
+    <definedName name="h_per_year">#REF!</definedName>
+    <definedName name="i">#REF!</definedName>
+    <definedName name="n">#REF!</definedName>
+    <definedName name="ProductionRate">[3]Summary!$C$8</definedName>
+  </definedNames>
   <calcPr calcId="181029" iterate="1" iterateCount="5000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,8 +65,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{4A486B45-271F-D245-BBE4-08B881A71805}" name="configuration" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/timothyw/Github Local/OpenPinch/OpenPinch/lib/configuration.txt" delimiter=":">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
   <si>
     <t>Process Zone</t>
   </si>
@@ -420,6 +462,138 @@
   </si>
   <si>
     <t>Cold</t>
+  </si>
+  <si>
+    <t>### General parameters ###</t>
+  </si>
+  <si>
+    <t>Value (blank = default value)</t>
+  </si>
+  <si>
+    <t>TOP_ZONE_NAME</t>
+  </si>
+  <si>
+    <t>TOP_ZONE_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>DT_CONT</t>
+  </si>
+  <si>
+    <t>DT_PHASE_CHANGE</t>
+  </si>
+  <si>
+    <t>T_ENV</t>
+  </si>
+  <si>
+    <t>DT_ENV_CONT</t>
+  </si>
+  <si>
+    <t>P_ENV</t>
+  </si>
+  <si>
+    <t>DECIMAL_PLACES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Targeting analysis flags ### </t>
+  </si>
+  <si>
+    <t>DO_DIRECT_OPERATION_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_DIRECT_SITE_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_INDIRECT_PROCESS_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_BALANCED_CC</t>
+  </si>
+  <si>
+    <t>DO_AREA_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_PROCESS_HP_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_UTILITY_HP_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_TURBINE_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_EXERGY_TARGETING</t>
+  </si>
+  <si>
+    <t>DO_VERTICAL_GCC</t>
+  </si>
+  <si>
+    <t>DO_ASSITED_HT</t>
+  </si>
+  <si>
+    <t>DO_TURBINE_WORK</t>
+  </si>
+  <si>
+    <t>### Heat pump targeting parameters ###</t>
+  </si>
+  <si>
+    <t>HP_TYPE</t>
+  </si>
+  <si>
+    <t>HP_LOAD_FRACTION</t>
+  </si>
+  <si>
+    <t>REFRIGERANTS</t>
+  </si>
+  <si>
+    <t>PRICE_RATIO_ELE_TO_FUEL</t>
+  </si>
+  <si>
+    <t>MAX_HP_MULTISTART</t>
+  </si>
+  <si>
+    <t>N_COND</t>
+  </si>
+  <si>
+    <t>N_EVAP</t>
+  </si>
+  <si>
+    <t>ETA_COMP</t>
+  </si>
+  <si>
+    <t>ETA_EXP</t>
+  </si>
+  <si>
+    <t>ETA_HP_CARNOT</t>
+  </si>
+  <si>
+    <t>ETA_HE_CARNOT</t>
+  </si>
+  <si>
+    <t>DTMIN_HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Cost targeting parameters ### </t>
+  </si>
+  <si>
+    <t>UTILITY_PRICE</t>
+  </si>
+  <si>
+    <t>ANNUAL_OP_TIME</t>
+  </si>
+  <si>
+    <t>FIXED_COST</t>
+  </si>
+  <si>
+    <t>VARIABLE_COST</t>
+  </si>
+  <si>
+    <t>COST_EXP</t>
+  </si>
+  <si>
+    <t>DISCOUNT_RATE</t>
+  </si>
+  <si>
+    <t>SERV_LIFE</t>
   </si>
 </sst>
 </file>
@@ -504,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -520,17 +694,18 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,6 +722,185 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Summary"/>
+      <sheetName val="Stream Data"/>
+      <sheetName val="Derivatives"/>
+      <sheetName val="Record"/>
+      <sheetName val="Utility Data"/>
+      <sheetName val="PT"/>
+      <sheetName val="CC"/>
+      <sheetName val="SCC"/>
+      <sheetName val="GCC"/>
+      <sheetName val="BCC"/>
+      <sheetName val="GCC (NP)"/>
+      <sheetName val="GCC (Ext)"/>
+      <sheetName val="GCC (Act)"/>
+      <sheetName val="ETD"/>
+      <sheetName val="HSDT"/>
+      <sheetName val="TSP"/>
+      <sheetName val="Input HEN"/>
+      <sheetName val="Grid"/>
+      <sheetName val="Example_ART_Input"/>
+      <sheetName val="Test Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Test Data"/>
+      <sheetName val="Summary"/>
+      <sheetName val="Stream Data"/>
+      <sheetName val="Record"/>
+      <sheetName val="Utility Data"/>
+      <sheetName val="PT"/>
+      <sheetName val="CC"/>
+      <sheetName val="SCC"/>
+      <sheetName val="GCC"/>
+      <sheetName val="BCC"/>
+      <sheetName val="GCC (NP)"/>
+      <sheetName val="GCC (Ext)"/>
+      <sheetName val="GCC (Act)"/>
+      <sheetName val="ETD"/>
+      <sheetName val="HSDT"/>
+      <sheetName val="TSP"/>
+      <sheetName val="NLC"/>
+      <sheetName val="xBCC"/>
+      <sheetName val="xGCC"/>
+      <sheetName val="xNLC"/>
+      <sheetName val="Multi-output"/>
+      <sheetName val="Options"/>
+      <sheetName val="License"/>
+      <sheetName val="Input HEN"/>
+      <sheetName val="Grid"/>
+      <sheetName val="Example_ART_Input"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="JSteamHidden"/>
+      <sheetName val="Summary"/>
+      <sheetName val="Stream Data"/>
+      <sheetName val="Separation"/>
+      <sheetName val="RO"/>
+      <sheetName val="Evaporator"/>
+      <sheetName val="Homogenisation"/>
+      <sheetName val="Spray Dryer"/>
+      <sheetName val="Record"/>
+      <sheetName val="Climate Data"/>
+      <sheetName val="Gas Turbine"/>
+      <sheetName val="Boiler"/>
+      <sheetName val="Electrical Model"/>
+      <sheetName val="Chiller"/>
+      <sheetName val="Reverse Brayton HP"/>
+      <sheetName val="Thermomechanical VR"/>
+      <sheetName val="Absorption Refrigeration"/>
+      <sheetName val="Info"/>
+      <sheetName val="Compositions"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="8">
+          <cell r="C8">
+            <v>10</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="configuration" connectionId="1" xr16:uid="{89A5A300-5D83-FF42-A67A-584B13DE0A8D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,14 +1231,15 @@
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -904,8 +1259,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
@@ -929,19 +1284,19 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>82.7</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>77.8</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>4613.0070000000051</v>
       </c>
-      <c r="F3" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="F3" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G3" s="7">
         <v>1</v>
       </c>
     </row>
@@ -952,19 +1307,19 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>83.2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>71.5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>9215.9730000000036</v>
       </c>
-      <c r="F4" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="F4" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="7">
         <v>1</v>
       </c>
     </row>
@@ -975,19 +1330,19 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>99.7</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>90.1</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>292.99200000000025</v>
       </c>
-      <c r="F5" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="F5" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -998,19 +1353,19 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>81.2</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>83.3</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>292.99199999999922</v>
       </c>
-      <c r="F6" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="F6" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1021,19 +1376,19 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>1.9</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>46.5</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>14337.116</v>
       </c>
-      <c r="F7" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="F7" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1044,19 +1399,19 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>1.9</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>65</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>17729.838</v>
       </c>
-      <c r="F8" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="F8" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1067,19 +1422,19 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>148.4</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>148.5</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>9747.9999999994452</v>
       </c>
-      <c r="F9" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G9" s="9">
+      <c r="F9" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1090,19 +1445,19 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>184.8</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>184.9</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>1497.999999999915</v>
       </c>
-      <c r="F10" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="F10" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1113,19 +1468,19 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>184.8</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>184.9</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>3051.9999999998263</v>
       </c>
-      <c r="F11" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="F11" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1136,19 +1491,19 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>97.1</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>87.6</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>2321.9899999999998</v>
       </c>
-      <c r="F12" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="F12" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G12" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1159,19 +1514,19 @@
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>148.4</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>148.5</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>864.99999999995089</v>
       </c>
-      <c r="F13" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="F13" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1182,19 +1537,19 @@
       <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>1.9</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>70</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>939.78</v>
       </c>
-      <c r="F14" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="F14" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1205,19 +1560,19 @@
       <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>84.1</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>68.400000000000006</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>6353.0049999999947</v>
       </c>
-      <c r="F15" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="F15" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1228,19 +1583,19 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>103.3</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <v>103.2</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>16584.999999999058</v>
       </c>
-      <c r="F16" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="F16" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G16" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1251,19 +1606,19 @@
       <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>80</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>74.3</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>6040.9740000000029</v>
       </c>
-      <c r="F17" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="F17" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1274,19 +1629,19 @@
       <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>165.4</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>146.5</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>1787.9400000000005</v>
       </c>
-      <c r="F18" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G18" s="9">
+      <c r="F18" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1297,19 +1652,19 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>90.8</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <v>108.1</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>1787.9549999999997</v>
       </c>
-      <c r="F19" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G19" s="9">
+      <c r="F19" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1320,19 +1675,19 @@
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>70.599999999999994</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>80</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>2235.0380000000014</v>
       </c>
-      <c r="F20" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G20" s="9">
+      <c r="F20" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G20" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1343,19 +1698,19 @@
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>184.8</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>184.9</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>20199.99999999885</v>
       </c>
-      <c r="F21" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G21" s="9">
+      <c r="F21" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1366,19 +1721,19 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>148.4</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="7">
         <v>148.5</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>3469.9999999998026</v>
       </c>
-      <c r="F22" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G22" s="9">
+      <c r="F22" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G22" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1389,19 +1744,19 @@
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>90.1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>50.5</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>1119.8879999999999</v>
       </c>
-      <c r="F23" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G23" s="9">
+      <c r="F23" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G23" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1412,19 +1767,19 @@
       <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>76.8</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="7">
         <v>53.6</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>19146.031999999996</v>
       </c>
-      <c r="F24" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G24" s="9">
+      <c r="F24" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1435,19 +1790,19 @@
       <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="7">
         <v>105.4</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="7">
         <v>111.9</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="7">
         <v>4128.0200000000004</v>
       </c>
-      <c r="F25" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="F25" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1458,19 +1813,19 @@
       <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>37.700000000000003</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="7">
         <v>50</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>702.94499999999982</v>
       </c>
-      <c r="F26" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G26" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1481,19 +1836,19 @@
       <c r="B27" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="7">
         <v>65</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="7">
         <v>75</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="7">
         <v>200</v>
       </c>
-      <c r="F27" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G27" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1504,19 +1859,19 @@
       <c r="B28" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="7">
         <v>49.2</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="7">
         <v>54.7</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="7">
         <v>42.019999999999996</v>
       </c>
-      <c r="F28" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G28" s="9">
+      <c r="F28" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G28" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1527,19 +1882,19 @@
       <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="7">
         <v>148.4</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="7">
         <v>148.5</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>3675.9999999997908</v>
       </c>
-      <c r="F29" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G29" s="9">
+      <c r="F29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G29" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1550,19 +1905,19 @@
       <c r="B30" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="7">
         <v>148.4</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>148.5</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>51792.999999997053</v>
       </c>
-      <c r="F30" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G30" s="9">
+      <c r="F30" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G30" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1573,19 +1928,19 @@
       <c r="B31" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <v>66.3</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>66.2</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>39394.999999997759</v>
       </c>
-      <c r="F31" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G31" s="9">
+      <c r="F31" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G31" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1596,19 +1951,19 @@
       <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="7">
         <v>65</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="7">
         <v>36</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="7">
         <v>3794.9400000000005</v>
       </c>
-      <c r="F32" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G32" s="9">
+      <c r="F32" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G32" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1619,19 +1974,19 @@
       <c r="B33" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="7">
         <v>53.6</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="7">
         <v>36</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="7">
         <v>14427.072000000002</v>
       </c>
-      <c r="F33" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G33" s="9">
+      <c r="F33" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G33" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1642,19 +1997,19 @@
       <c r="B34" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="7">
         <v>88.3</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="7">
         <v>7319.2</v>
       </c>
-      <c r="F34" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="F34" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G34" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1665,19 +2020,19 @@
       <c r="B35" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="7">
         <v>99.6</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <v>99.5</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <v>717.99999999995919</v>
       </c>
-      <c r="F35" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F35" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G35" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1688,19 +2043,19 @@
       <c r="B36" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="7">
         <v>148.4</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="7">
         <v>148.5</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <v>1105.9999999999372</v>
       </c>
-      <c r="F36" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G36" s="9">
+      <c r="F36" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G36" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1711,19 +2066,19 @@
       <c r="B37" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="7">
         <v>40.200000000000003</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="7">
         <v>40.1</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="7">
         <v>581.0000000000083</v>
       </c>
-      <c r="F37" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G37" s="9">
+      <c r="F37" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G37" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1734,19 +2089,19 @@
       <c r="B38" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="7">
         <v>1.9</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="7">
         <v>20</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="7">
         <v>3368.0480000000007</v>
       </c>
-      <c r="F38" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G38" s="9">
+      <c r="F38" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G38" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1757,19 +2112,19 @@
       <c r="B39" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="7">
         <v>104</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <v>59</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="7">
         <v>3599.1000000000004</v>
       </c>
-      <c r="F39" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G39" s="9">
+      <c r="F39" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G39" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1780,19 +2135,19 @@
       <c r="B40" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="7">
         <v>59</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="7">
         <v>50</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="7">
         <v>8966.9700000000012</v>
       </c>
-      <c r="F40" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G40" s="9">
+      <c r="F40" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G40" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1803,19 +2158,19 @@
       <c r="B41" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="7">
         <v>129.1</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="7">
         <v>129</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="7">
         <v>1394.9999999999206</v>
       </c>
-      <c r="F41" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G41" s="9">
+      <c r="F41" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G41" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1826,19 +2181,19 @@
       <c r="B42" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="7">
         <v>120.2</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="7">
         <v>120.1</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="7">
         <v>2808.0000000002392</v>
       </c>
-      <c r="F42" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G42" s="9">
+      <c r="F42" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G42" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1849,19 +2204,19 @@
       <c r="B43" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="7">
         <v>36.799999999999997</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="7">
         <v>122.7</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="7">
         <v>9881.9360000000015</v>
       </c>
-      <c r="F43" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G43" s="9">
+      <c r="F43" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G43" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1872,19 +2227,19 @@
       <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="7">
         <v>4.3</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="7">
         <v>148.30000000000001</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="7">
         <v>10945.44</v>
       </c>
-      <c r="F44" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="F44" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G44" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1895,19 +2250,19 @@
       <c r="B45" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="7">
         <v>3</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="7">
         <v>34.9</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="7">
         <v>498.916</v>
       </c>
-      <c r="F45" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G45" s="9">
+      <c r="F45" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G45" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1918,19 +2273,19 @@
       <c r="B46" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="7">
         <v>3</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="7">
         <v>36.799999999999997</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="7">
         <v>2073.9679999999998</v>
       </c>
-      <c r="F46" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G46" s="9">
+      <c r="F46" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G46" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1941,19 +2296,19 @@
       <c r="B47" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="7">
         <v>52</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="7">
         <v>70</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="7">
         <v>2808</v>
       </c>
-      <c r="F47" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="F47" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G47" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1964,19 +2319,19 @@
       <c r="B48" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="7">
         <v>148.4</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="7">
         <v>148.5</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="7">
         <v>21689.999999998767</v>
       </c>
-      <c r="F48" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G48" s="9">
+      <c r="F48" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G48" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1987,19 +2342,19 @@
       <c r="B49" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="7">
         <v>148.4</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="7">
         <v>148.5</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="7">
         <v>2875.9999999998363</v>
       </c>
-      <c r="F49" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G49" s="9">
+      <c r="F49" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G49" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2010,19 +2365,19 @@
       <c r="B50" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="7">
         <v>2.7</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="7">
         <v>52.1</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="7">
         <v>7730.1119999999992</v>
       </c>
-      <c r="F50" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G50" s="9">
+      <c r="F50" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G50" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2033,19 +2388,19 @@
       <c r="B51" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="7">
         <v>1.9</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="7">
         <v>45</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="7">
         <v>3419.123</v>
       </c>
-      <c r="F51" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G51" s="9">
+      <c r="F51" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G51" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2056,19 +2411,19 @@
       <c r="B52" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="7">
         <v>83</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="7">
         <v>106.2</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="7">
         <v>9883.8960000000006</v>
       </c>
-      <c r="F52" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G52" s="9">
+      <c r="F52" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G52" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2079,19 +2434,19 @@
       <c r="B53" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="7">
         <v>204.5</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="7">
         <v>133.19999999999999</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="7">
         <v>9884.3190000000013</v>
       </c>
-      <c r="F53" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G53" s="9">
+      <c r="F53" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G53" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2102,19 +2457,19 @@
       <c r="B54" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="7">
         <v>16.100000000000001</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="7">
         <v>17</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="7">
         <v>134.00099999999978</v>
       </c>
-      <c r="F54" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G54" s="9">
+      <c r="F54" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G54" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2125,19 +2480,19 @@
       <c r="B55" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="7">
         <v>148.4</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="7">
         <v>148.5</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="7">
         <v>13126.999999999254</v>
       </c>
-      <c r="F55" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G55" s="9">
+      <c r="F55" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G55" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2148,19 +2503,19 @@
       <c r="B56" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="7">
         <v>148.80000000000001</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="7">
         <v>148.9</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="7">
         <v>11766.999999999331</v>
       </c>
-      <c r="F56" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G56" s="9">
+      <c r="F56" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G56" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2171,19 +2526,19 @@
       <c r="B57" t="s">
         <v>80</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="7">
         <v>148.4</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="7">
         <v>148.5</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="7">
         <v>6351.9999999996389</v>
       </c>
-      <c r="F57" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G57" s="9">
+      <c r="F57" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G57" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2194,19 +2549,19 @@
       <c r="B58" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="7">
         <v>184.8</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="7">
         <v>184.9</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="7">
         <v>4334.9999999997535</v>
       </c>
-      <c r="F58" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G58" s="9">
+      <c r="F58" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G58" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2217,19 +2572,19 @@
       <c r="B59" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="7">
         <v>117.8</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="7">
         <v>84.4</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="7">
         <v>11773.833999999997</v>
       </c>
-      <c r="F59" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G59" s="9">
+      <c r="F59" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G59" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2240,19 +2595,19 @@
       <c r="B60" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="7">
         <v>66.8</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="7">
         <v>107.7</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="7">
         <v>6287.9660000000013</v>
       </c>
-      <c r="F60" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G60" s="9">
+      <c r="F60" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G60" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2263,19 +2618,19 @@
       <c r="B61" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="7">
         <v>63.8</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="7">
         <v>102.9</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="7">
         <v>5486.121000000001</v>
       </c>
-      <c r="F61" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G61" s="9">
+      <c r="F61" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G61" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2286,19 +2641,19 @@
       <c r="B62" t="s">
         <v>86</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="7">
         <v>148.4</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="7">
         <v>148.5</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="7">
         <v>804.9999999999543</v>
       </c>
-      <c r="F62" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G62" s="9">
+      <c r="F62" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G62" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2309,19 +2664,19 @@
       <c r="B63" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="7">
         <v>148.4</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="7">
         <v>148.5</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="7">
         <v>3006.999999999829</v>
       </c>
-      <c r="F63" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G63" s="9">
+      <c r="F63" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G63" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2332,19 +2687,19 @@
       <c r="B64" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="7">
         <v>87</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="7">
         <v>78</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E64" s="7">
         <v>4506.03</v>
       </c>
-      <c r="F64" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G64" s="9">
+      <c r="F64" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G64" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2355,19 +2710,19 @@
       <c r="B65" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="7">
         <v>87</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D65" s="7">
         <v>82</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E65" s="7">
         <v>1068</v>
       </c>
-      <c r="F65" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G65" s="9">
+      <c r="F65" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G65" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2378,19 +2733,19 @@
       <c r="B66" t="s">
         <v>91</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="7">
         <v>67.900000000000006</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D66" s="7">
         <v>38.299999999999997</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="7">
         <v>4090.1280000000015</v>
       </c>
-      <c r="F66" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="G66" s="9">
+      <c r="F66" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G66" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2412,7 +2767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229D93BF-F0F2-F747-8102-E6B7A5EB8F25}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2423,10 +2778,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -2446,8 +2801,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
@@ -2465,10 +2820,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="3">
@@ -2488,10 +2843,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="3">
@@ -2511,10 +2866,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>95</v>
       </c>
       <c r="C5" s="3">
@@ -2534,10 +2889,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="3">
@@ -2574,4 +2929,247 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7EE7E0-8CC0-0B49-AC08-EF1AF9C010A9}">
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>